<commit_message>
pred pridanim LOGGED stavu do app.ts
</commit_message>
<xml_diff>
--- a/Web4/BlendedAPI/vyzva/Server/Excels/StudyAll.xlsx
+++ b/Web4/BlendedAPI/vyzva/Server/Excels/StudyAll.xlsx
@@ -9,14 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="studydetails" sheetId="1" r:id="rId1"/>
     <sheet name="studyblocks" sheetId="3" r:id="rId2"/>
-    <sheet name="Studijní bloky" sheetId="4" r:id="rId3"/>
-    <sheet name="Přehled" sheetId="2" r:id="rId4"/>
-    <sheet name="Detaily" sheetId="5" r:id="rId5"/>
+    <sheet name="Studijní bloky - počet" sheetId="4" r:id="rId3"/>
+    <sheet name="Studijní bloky - procenta" sheetId="6" r:id="rId4"/>
+    <sheet name="Přehled Studijních skupin" sheetId="2" r:id="rId5"/>
+    <sheet name="Detaily dle Studijnch skupin" sheetId="5" r:id="rId6"/>
+    <sheet name="Detaily dle Studentů" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="studyblocks" localSheetId="1">studyblocks!$A$1:$D$2</definedName>
@@ -24,8 +26,8 @@
   </definedNames>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="8" r:id="rId6"/>
-    <pivotCache cacheId="13" r:id="rId7"/>
+    <pivotCache cacheId="8" r:id="rId8"/>
+    <pivotCache cacheId="13" r:id="rId9"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,13 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="32">
-  <si>
-    <t>Přehrání nahrávek</t>
-  </si>
-  <si>
-    <t>Přehrání zvuku</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="30">
   <si>
     <t>English</t>
   </si>
@@ -101,18 +97,9 @@
     <t>Čas výuky</t>
   </si>
   <si>
-    <t>Nahrávek</t>
-  </si>
-  <si>
     <t>sss</t>
   </si>
   <si>
-    <t>Celkem Počet</t>
-  </si>
-  <si>
-    <t>Celkem Procent</t>
-  </si>
-  <si>
     <t>Počet</t>
   </si>
   <si>
@@ -132,6 +119,15 @@
   </si>
   <si>
     <t>_learnphase</t>
+  </si>
+  <si>
+    <t>Vlastní nahrávky</t>
+  </si>
+  <si>
+    <t>Přehráno nahrávek</t>
+  </si>
+  <si>
+    <t>Přehráno zvuku</t>
   </si>
 </sst>
 </file>
@@ -174,7 +170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -199,11 +195,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="14">
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="31" formatCode="[h]:mm:ss"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="31" formatCode="[h]:mm:ss"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="31" formatCode="[h]:mm:ss"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="31" formatCode="[h]:mm:ss"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="31" formatCode="[h]:mm:ss"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="31" formatCode="[h]:mm:ss"/>
     </dxf>
@@ -230,7 +257,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="pavel pz." refreshedDate="42260.387558101851" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="2">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="pavel pz." refreshedDate="42260.66781111111" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="2">
   <cacheSource type="worksheet">
     <worksheetSource name="studydetails" sheet="studydetails"/>
   </cacheSource>
@@ -293,7 +320,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="pavel pz." refreshedDate="42260.387558449074" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="pavel pz." refreshedDate="42260.667811689818" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="1">
   <cacheSource type="worksheet">
     <worksheetSource name="studyblocks" sheet="studyblocks"/>
   </cacheSource>
@@ -370,7 +397,7 @@
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Kontingenční tabulka 1" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Hodnoty" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
-  <location ref="B10:F14" firstHeaderRow="0" firstDataRow="2" firstDataCol="1"/>
+  <location ref="B10:D14" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField dataField="1" showAll="0" defaultSubtotal="0"/>
     <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
@@ -405,27 +432,78 @@
       <x/>
     </i>
   </rowItems>
-  <colFields count="2">
+  <colFields count="1">
     <field x="3"/>
-    <field x="-2"/>
   </colFields>
-  <colItems count="4">
+  <colItems count="2">
     <i>
       <x/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
     </i>
     <i t="grand">
       <x/>
     </i>
-    <i t="grand" i="1">
-      <x/>
-    </i>
   </colItems>
-  <dataFields count="2">
+  <dataFields count="1">
     <dataField name="Počet" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Kontingenční tabulka 1" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Hodnoty" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+  <location ref="B10:D14" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="5">
+    <pivotField dataField="1" showAll="0" defaultSubtotal="0"/>
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="1">
+        <item x="0"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0" sortType="ascending" defaultSubtotal="0">
+      <items count="1">
+        <item x="0"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
+      <items count="1">
+        <item x="0"/>
+      </items>
+    </pivotField>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="2"/>
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="3"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
     <dataField name="Procent" fld="0" subtotal="count" showDataAs="percentOfRow" baseField="2" baseItem="0" numFmtId="10"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
@@ -437,7 +515,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Kontingenční tabulka 3" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Hodnoty" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
   <location ref="B10:G14" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
@@ -504,12 +582,12 @@
   <dataFields count="5">
     <dataField name="Skore" fld="11" baseField="0" baseItem="0" numFmtId="9"/>
     <dataField name="Čas výuky" fld="7" baseField="2" baseItem="0" numFmtId="46"/>
-    <dataField name="Nahrávek" fld="8" baseField="2" baseItem="0" numFmtId="46"/>
-    <dataField name="Přehrání nahrávek" fld="9" baseField="2" baseItem="0" numFmtId="46"/>
-    <dataField name="Přehrání zvuku" fld="10" baseField="2" baseItem="0" numFmtId="46"/>
+    <dataField name="Vlastní nahrávky" fld="8" baseField="2" baseItem="0" numFmtId="46"/>
+    <dataField name="Přehráno nahrávek" fld="9" baseField="2" baseItem="0" numFmtId="46"/>
+    <dataField name="Přehráno zvuku" fld="10" baseField="2" baseItem="0" numFmtId="46"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="3">
+    <format dxfId="13">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -518,7 +596,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="2">
+    <format dxfId="12">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="4" selected="0">
@@ -540,7 +618,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Kontingenční tabulka 2" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Hodnoty" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
   <location ref="B10:G17" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
@@ -634,12 +712,12 @@
   <dataFields count="5">
     <dataField name="Skore" fld="11" baseField="0" baseItem="0" numFmtId="9"/>
     <dataField name="Čas výuky" fld="7" baseField="2" baseItem="0" numFmtId="46"/>
-    <dataField name="Nahrávek" fld="8" baseField="2" baseItem="0" numFmtId="46"/>
-    <dataField name="Přehrání nahrávek" fld="9" baseField="2" baseItem="0" numFmtId="46"/>
-    <dataField name="Přehrání zvuku" fld="10" baseField="2" baseItem="0" numFmtId="46"/>
+    <dataField name="Vlastní nahrávky" fld="8" baseField="2" baseItem="0" numFmtId="46"/>
+    <dataField name="Přehráno nahrávek" fld="9" baseField="2" baseItem="0" numFmtId="46"/>
+    <dataField name="Přehráno zvuku" fld="10" baseField="2" baseItem="0" numFmtId="46"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="1">
+    <format dxfId="11">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -648,7 +726,132 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="0">
+    <format dxfId="10">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="4" selected="0">
+            <x v="1"/>
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Kontingenční tabulka 2" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Hodnoty" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+  <location ref="B10:G16" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="12">
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="2">
+        <item x="0"/>
+        <item x="1"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0" sortType="ascending" defaultSubtotal="0">
+      <items count="2">
+        <item x="0"/>
+        <item sd="0" x="1"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0" sortType="ascending" defaultSubtotal="0">
+      <items count="1">
+        <item x="0"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="2">
+        <item x="1"/>
+        <item x="0"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0" sortType="ascending" defaultSubtotal="0">
+      <items count="2">
+        <item x="1"/>
+        <item x="0"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="1" showAll="0" defaultSubtotal="0"/>
+    <pivotField numFmtId="1" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" numFmtId="46" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" numFmtId="46" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" numFmtId="46" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" numFmtId="46" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="3">
+    <field x="2"/>
+    <field x="3"/>
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+    <i i="3">
+      <x v="3"/>
+    </i>
+    <i i="4">
+      <x v="4"/>
+    </i>
+  </colItems>
+  <dataFields count="5">
+    <dataField name="Skore" fld="11" baseField="0" baseItem="0" numFmtId="9"/>
+    <dataField name="Čas výuky" fld="7" baseField="2" baseItem="0" numFmtId="46"/>
+    <dataField name="Vlastní nahrávky" fld="8" baseField="2" baseItem="0" numFmtId="46"/>
+    <dataField name="Přehráno nahrávek" fld="9" baseField="2" baseItem="0" numFmtId="46"/>
+    <dataField name="Přehráno zvuku" fld="10" baseField="2" baseItem="0" numFmtId="46"/>
+  </dataFields>
+  <formats count="2">
+    <format dxfId="4">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="5">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="4" selected="0">
@@ -947,54 +1150,54 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>4</v>
       </c>
       <c r="F2" s="3">
         <v>400</v>
@@ -1017,19 +1220,19 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F3" s="3">
         <v>0</v>
@@ -1139,30 +1342,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1172,80 +1375,60 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B10:F14"/>
+  <dimension ref="B10:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="6" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" customWidth="1"/>
+    <col min="3" max="3" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.5703125" customWidth="1"/>
     <col min="6" max="6" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C12" s="8"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="9"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D12" s="8"/>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C13" s="8">
         <v>1</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="8">
         <v>1</v>
       </c>
-      <c r="E13" s="8">
-        <v>1</v>
-      </c>
-      <c r="F13" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C14" s="8">
         <v>1</v>
       </c>
-      <c r="D14" s="9">
-        <v>1</v>
-      </c>
-      <c r="E14" s="8">
-        <v>1</v>
-      </c>
-      <c r="F14" s="9">
+      <c r="D14" s="8">
         <v>1</v>
       </c>
     </row>
@@ -1256,10 +1439,74 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B10:D14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="9">
+        <v>1</v>
+      </c>
+      <c r="D13" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="9">
+        <v>1</v>
+      </c>
+      <c r="D14" s="9">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B10:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1267,31 +1514,31 @@
     <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6" customWidth="1"/>
     <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E10" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="F10" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="G10" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="6"/>
@@ -1301,7 +1548,7 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C12" s="7">
         <v>0.75</v>
@@ -1321,7 +1568,7 @@
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="10" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C13" s="7">
         <v>0</v>
@@ -1341,7 +1588,7 @@
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C14" s="7">
         <v>0.75</v>
@@ -1364,12 +1611,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B10:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J25" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1377,31 +1624,31 @@
     <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6" customWidth="1"/>
     <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E10" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="F10" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="G10" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="6"/>
@@ -1411,7 +1658,7 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="6"/>
@@ -1421,7 +1668,7 @@
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="11" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="6"/>
@@ -1431,7 +1678,7 @@
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="12" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="6"/>
@@ -1441,7 +1688,7 @@
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="13" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C15" s="7">
         <v>0.75</v>
@@ -1461,7 +1708,7 @@
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="10" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C16" s="7">
         <v>0</v>
@@ -1481,7 +1728,7 @@
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C17" s="7">
         <v>0.75</v>
@@ -1496,6 +1743,136 @@
         <v>0.18055555555555555</v>
       </c>
       <c r="G17" s="6">
+        <v>0.2638888888888889</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B10:G16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="7"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="7">
+        <v>0</v>
+      </c>
+      <c r="D13" s="6">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="E13" s="6">
+        <v>4.8611111111111112E-2</v>
+      </c>
+      <c r="F13" s="6">
+        <v>9.0277777777777776E-2</v>
+      </c>
+      <c r="G13" s="6">
+        <v>0.13194444444444445</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="7">
+        <v>0.75</v>
+      </c>
+      <c r="D15" s="6">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="E15" s="6">
+        <v>4.8611111111111112E-2</v>
+      </c>
+      <c r="F15" s="6">
+        <v>9.0277777777777776E-2</v>
+      </c>
+      <c r="G15" s="6">
+        <v>0.13194444444444445</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="7">
+        <v>0.75</v>
+      </c>
+      <c r="D16" s="6">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="E16" s="6">
+        <v>9.7222222222222224E-2</v>
+      </c>
+      <c r="F16" s="6">
+        <v>0.18055555555555555</v>
+      </c>
+      <c r="G16" s="6">
         <v>0.2638888888888889</v>
       </c>
     </row>

</xml_diff>

<commit_message>
vyzva web a opravy
</commit_message>
<xml_diff>
--- a/Web4/BlendedAPI/vyzva/Server/Excels/StudyAll.xlsx
+++ b/Web4/BlendedAPI/vyzva/Server/Excels/StudyAll.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="1000" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="1000" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="studydetails" sheetId="1" state="hidden" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="63">
   <si>
     <t>Celkový součet</t>
   </si>
@@ -143,28 +143,13 @@
     <t>Důležité upozornění: Před započetím práce s tímto souborem je potřeba kliknout na tlačítko "Povolit úpravy" nahoře na obrazovce.</t>
   </si>
   <si>
-    <t>V tomto souboru naleznete aktuální přehledné i detailní informace o průběhu studia.</t>
-  </si>
-  <si>
-    <t>TIP: rozbalte x sbalte údaje pomocí malých tlačítek + nebo -. Získáte tak kumulované x detailní informace.</t>
-  </si>
-  <si>
     <t>TIP: dvojklikem (poklepáním) na čísla v tabulce se vám na novém listu ukáže detailní seznam údajů, na základě kterých bylo číslo vypočítáno</t>
-  </si>
-  <si>
-    <t>Význam některých sloupců v poskytnutých tabulkách</t>
   </si>
   <si>
     <t>Název sloupce</t>
   </si>
   <si>
     <t>Význam</t>
-  </si>
-  <si>
-    <t>Skore</t>
-  </si>
-  <si>
-    <t>Průměrné skore za všechna vyhodnotitelná cvičení.</t>
   </si>
   <si>
     <t>Celkový čas, strávený výukou</t>
@@ -209,9 +194,6 @@
     <t>Údaje jsou seskupeny dle Kurzu =&gt; Studijní skupiny</t>
   </si>
   <si>
-    <t>Údaje jsou seskupeny dle Kurzu =&gt; Studijní skupiny =&gt; Kurzu =&gt; Jazykové úrovně =&gt; Studenta</t>
-  </si>
-  <si>
     <t>Kolik procent cvičení z celého kurzu student odstudoval</t>
   </si>
   <si>
@@ -226,6 +208,28 @@
   <si>
     <t>Tabulka měří procento studentů, kteří dosáhli určitého pokroku v této sedmiprvkové posloupnosti:</t>
   </si>
+  <si>
+    <t>V tomto souboru naleznete aktuální souhrnné i detailní informace o průběhu studia.</t>
+  </si>
+  <si>
+    <t>TIP 2: rozbalte x sbalte údaje pomocí malých tlačítek + nebo -. Získáte tak kumulované x detailní informace.</t>
+  </si>
+  <si>
+    <t>TIP 3: dvojklikem (poklepáním) na čísla v tabulce se vám na novém listu ukáže detailní seznam údajů, na základě kterých bylo číslo vypočítáno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TIP 1: postupně procházejte jednotlivé přehledové tabulky, klikáním na záložky ve spodní části okna.
+</t>
+  </si>
+  <si>
+    <t>Průměrné skóre za všechna vyhodnotitelná cvičení.</t>
+  </si>
+  <si>
+    <t>Význam některých sloupců v tabulkách na následujících listech</t>
+  </si>
+  <si>
+    <t>Údaje jsou seskupeny dle Kurzu =&gt; Studijní skupiny =&gt; Jazykové úrovně =&gt; Lekce/Testu =&gt; Studenta</t>
+  </si>
 </sst>
 </file>
 
@@ -234,7 +238,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -316,12 +320,6 @@
       <color theme="4"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -699,13 +697,40 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="LM Normální" xfId="1"/>
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="60">
+  <dxfs count="68">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0%"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
     </dxf>
@@ -1385,9 +1410,6 @@
       <font>
         <b/>
       </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0%"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0%"/>
@@ -2240,11 +2262,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="330690528"/>
-        <c:axId val="330689744"/>
+        <c:axId val="432205304"/>
+        <c:axId val="432211968"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="330690528"/>
+        <c:axId val="432205304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2287,7 +2309,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="330689744"/>
+        <c:crossAx val="432211968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2295,7 +2317,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="330689744"/>
+        <c:axId val="432211968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2346,7 +2368,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="330690528"/>
+        <c:crossAx val="432205304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -2602,11 +2624,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="330690136"/>
-        <c:axId val="330688176"/>
+        <c:axId val="432213144"/>
+        <c:axId val="432214712"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="330690136"/>
+        <c:axId val="432213144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2649,7 +2671,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="330688176"/>
+        <c:crossAx val="432214712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2657,7 +2679,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="330688176"/>
+        <c:axId val="432214712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2709,7 +2731,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="330690136"/>
+        <c:crossAx val="432213144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -3330,11 +3352,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="330683864"/>
-        <c:axId val="330685432"/>
+        <c:axId val="432207264"/>
+        <c:axId val="432211184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="330683864"/>
+        <c:axId val="432207264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3377,7 +3399,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="330685432"/>
+        <c:crossAx val="432211184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3385,7 +3407,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="330685432"/>
+        <c:axId val="432211184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3436,7 +3458,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="330683864"/>
+        <c:crossAx val="432207264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5262,7 +5284,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="pavel pz." refreshedDate="42264.65224236111" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="pavel pz." refreshedDate="42265.353114930556" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="1">
   <cacheSource type="worksheet">
     <worksheetSource name="studyblocks" sheet="studyblocks"/>
   </cacheSource>
@@ -5302,7 +5324,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="pavel pz." refreshedDate="42264.652243055556" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="2">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="pavel pz." refreshedDate="42265.353115625003" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="2">
   <cacheSource type="worksheet">
     <worksheetSource name="studydetails" sheet="studydetails"/>
   </cacheSource>
@@ -5694,7 +5716,7 @@
     <dataField name="Odstudováno" fld="14" baseField="0" baseItem="0" numFmtId="1"/>
   </dataFields>
   <formats count="20">
-    <format dxfId="59">
+    <format dxfId="67">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -5703,7 +5725,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="58">
+    <format dxfId="66">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="4" selected="0">
@@ -5715,7 +5737,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="57">
+    <format dxfId="65">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="4">
           <reference field="4294967294" count="1" selected="0">
@@ -5727,7 +5749,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="56">
+    <format dxfId="64">
       <pivotArea field="2" grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -5736,14 +5758,14 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="55">
+    <format dxfId="63">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="54">
+    <format dxfId="62">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="0" selected="0"/>
@@ -5753,7 +5775,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="53">
+    <format dxfId="61">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="3">
           <reference field="0" count="1">
@@ -5766,7 +5788,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="52">
+    <format dxfId="60">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="0" selected="0"/>
@@ -5776,7 +5798,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="51">
+    <format dxfId="59">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="3">
           <reference field="0" count="1">
@@ -5789,14 +5811,14 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="50">
+    <format dxfId="58">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="49">
+    <format dxfId="57">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="0" selected="0"/>
@@ -5804,14 +5826,14 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="48">
+    <format dxfId="56">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="47">
+    <format dxfId="55">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="0" selected="0"/>
@@ -5821,7 +5843,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="46">
+    <format dxfId="54">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="3">
           <reference field="0" count="1">
@@ -5834,7 +5856,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="45">
+    <format dxfId="53">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="0" selected="0"/>
@@ -5844,7 +5866,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="44">
+    <format dxfId="52">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="3">
           <reference field="0" count="1">
@@ -5857,14 +5879,14 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="43">
+    <format dxfId="51">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="42">
+    <format dxfId="50">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="0" selected="0"/>
@@ -5872,7 +5894,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="41">
+    <format dxfId="49">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="0" count="0"/>
@@ -5883,7 +5905,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="40">
+    <format dxfId="48">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="0" count="0"/>
@@ -5983,7 +6005,7 @@
     <dataField name="Odstudováno" fld="14" baseField="0" baseItem="0" numFmtId="1"/>
   </dataFields>
   <formats count="4">
-    <format dxfId="39">
+    <format dxfId="47">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -5992,7 +6014,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="38">
+    <format dxfId="46">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="4" selected="0">
@@ -6004,7 +6026,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="37">
+    <format dxfId="45">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="3">
           <reference field="4294967294" count="1" selected="0">
@@ -6015,7 +6037,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="36">
+    <format dxfId="44">
       <pivotArea field="2" grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -6275,8 +6297,8 @@
     <dataField name="Odstudovaných cvičení" fld="4" baseField="0" baseItem="0"/>
     <dataField name="Odstudováno" fld="14" baseField="0" baseItem="0" numFmtId="1"/>
   </dataFields>
-  <formats count="6">
-    <format dxfId="35">
+  <formats count="13">
+    <format dxfId="43">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -6285,7 +6307,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="34">
+    <format dxfId="42">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="4" selected="0">
@@ -6297,7 +6319,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="33">
+    <format dxfId="41">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="5">
           <reference field="4294967294" count="1" selected="0">
@@ -6310,16 +6332,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="32">
-      <pivotArea field="2" grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="31">
+    <format dxfId="40">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="1" count="0" selected="0"/>
@@ -6330,13 +6343,127 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="30">
+    <format dxfId="39">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="1" count="0" selected="0"/>
           <reference field="2" count="0" selected="0"/>
           <reference field="3" count="1">
             <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="8">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+          <reference field="1" count="0"/>
+          <reference field="2" count="0" selected="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="7">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="4">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+          <reference field="1" count="0" selected="0"/>
+          <reference field="2" count="0" selected="0"/>
+          <reference field="3" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="6">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="5">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+          <reference field="1" count="0" selected="0"/>
+          <reference field="2" count="0" selected="0"/>
+          <reference field="3" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="5">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="6">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+          <reference field="0" count="1">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="0" selected="0"/>
+          <reference field="2" count="0" selected="0"/>
+          <reference field="3" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="0" selected="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="4">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="4">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+          <reference field="1" count="0" selected="0"/>
+          <reference field="2" count="0" selected="0"/>
+          <reference field="3" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="3">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="5">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+          <reference field="1" count="0" selected="0"/>
+          <reference field="2" count="0" selected="0"/>
+          <reference field="3" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="5" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="2">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="6">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+          <reference field="0" count="1">
+            <x v="1"/>
+          </reference>
+          <reference field="1" count="0" selected="0"/>
+          <reference field="2" count="0" selected="0"/>
+          <reference field="3" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="5" count="0" selected="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="1">
+      <pivotArea field="2" grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="6"/>
           </reference>
         </references>
       </pivotArea>
@@ -6845,10 +6972,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T25"/>
+  <dimension ref="A1:T26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U26" sqref="U26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6905,7 +7032,7 @@
     </row>
     <row r="6" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B6" s="35" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="C6" s="36"/>
       <c r="D6" s="36"/>
@@ -6947,9 +7074,9 @@
       <c r="S7" s="23"/>
       <c r="T7" s="23"/>
     </row>
-    <row r="8" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="35" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="C8" s="36"/>
       <c r="D8" s="36"/>
@@ -6970,153 +7097,151 @@
       <c r="S8" s="23"/>
       <c r="T8" s="23"/>
     </row>
-    <row r="9" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="38" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39"/>
-      <c r="J9" s="39"/>
-      <c r="K9" s="39"/>
-      <c r="L9" s="39"/>
-      <c r="M9" s="39"/>
-      <c r="N9" s="39"/>
-      <c r="O9" s="39"/>
-      <c r="P9" s="39"/>
-      <c r="Q9" s="40"/>
+    <row r="9" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="36"/>
+      <c r="J9" s="36"/>
+      <c r="K9" s="36"/>
+      <c r="L9" s="36"/>
+      <c r="M9" s="36"/>
+      <c r="N9" s="36"/>
+      <c r="O9" s="36"/>
+      <c r="P9" s="36"/>
+      <c r="Q9" s="37"/>
       <c r="R9" s="23"/>
       <c r="S9" s="23"/>
       <c r="T9" s="23"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B10" s="57"/>
-      <c r="C10" s="57"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="57"/>
-      <c r="F10" s="57"/>
-      <c r="G10" s="57"/>
-      <c r="H10" s="57"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="57"/>
-      <c r="K10" s="57"/>
-      <c r="L10" s="57"/>
-      <c r="M10" s="57"/>
-      <c r="N10" s="57"/>
-      <c r="O10" s="57"/>
-      <c r="P10" s="57"/>
-      <c r="Q10" s="57"/>
+    <row r="10" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="39"/>
+      <c r="L10" s="39"/>
+      <c r="M10" s="39"/>
+      <c r="N10" s="39"/>
+      <c r="O10" s="39"/>
+      <c r="P10" s="39"/>
+      <c r="Q10" s="40"/>
       <c r="R10" s="23"/>
       <c r="S10" s="23"/>
       <c r="T10" s="23"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="57"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="24"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="24"/>
-      <c r="L11" s="24"/>
-      <c r="M11" s="24"/>
-      <c r="N11" s="24"/>
-      <c r="O11" s="24"/>
-      <c r="P11" s="24"/>
-      <c r="Q11" s="24"/>
-      <c r="R11" s="24"/>
+      <c r="B11" s="57"/>
+      <c r="C11" s="57"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="57"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="57"/>
+      <c r="L11" s="57"/>
+      <c r="M11" s="57"/>
+      <c r="N11" s="57"/>
+      <c r="O11" s="57"/>
+      <c r="P11" s="57"/>
+      <c r="Q11" s="57"/>
+      <c r="R11" s="23"/>
       <c r="S11" s="23"/>
-      <c r="T11" s="24"/>
-    </row>
-    <row r="12" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T11" s="23"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="57"/>
-      <c r="B12" s="58" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="58"/>
-      <c r="D12" s="58"/>
-      <c r="E12" s="58"/>
-      <c r="F12" s="58"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="25"/>
-      <c r="M12" s="25"/>
-      <c r="N12" s="25"/>
-      <c r="O12" s="25"/>
-      <c r="P12" s="25"/>
-      <c r="Q12" s="25"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="24"/>
+      <c r="N12" s="24"/>
+      <c r="O12" s="24"/>
+      <c r="P12" s="24"/>
+      <c r="Q12" s="24"/>
       <c r="R12" s="24"/>
       <c r="S12" s="23"/>
-      <c r="T12" s="23"/>
-    </row>
-    <row r="13" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="54" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="55"/>
-      <c r="D13" s="56" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="56"/>
-      <c r="F13" s="56"/>
-      <c r="G13" s="56"/>
-      <c r="H13" s="56"/>
-      <c r="I13" s="56"/>
-      <c r="J13" s="56"/>
-      <c r="K13" s="56"/>
-      <c r="L13" s="56"/>
-      <c r="M13" s="56"/>
-      <c r="N13" s="56"/>
-      <c r="O13" s="56"/>
-      <c r="P13" s="56"/>
-      <c r="Q13" s="55"/>
-      <c r="R13" s="25"/>
+      <c r="T12" s="24"/>
+    </row>
+    <row r="13" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="57"/>
+      <c r="B13" s="58" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="58"/>
+      <c r="D13" s="58"/>
+      <c r="E13" s="58"/>
+      <c r="F13" s="58"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="25"/>
+      <c r="L13" s="25"/>
+      <c r="M13" s="25"/>
+      <c r="N13" s="25"/>
+      <c r="O13" s="25"/>
+      <c r="P13" s="25"/>
+      <c r="Q13" s="25"/>
+      <c r="R13" s="24"/>
       <c r="S13" s="23"/>
       <c r="T13" s="23"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B14" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="27"/>
-      <c r="D14" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="24"/>
-      <c r="J14" s="24"/>
-      <c r="K14" s="24"/>
-      <c r="L14" s="24"/>
-      <c r="M14" s="24"/>
-      <c r="N14" s="24"/>
-      <c r="O14" s="24"/>
-      <c r="P14" s="24"/>
-      <c r="Q14" s="27"/>
+    <row r="14" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="55"/>
+      <c r="D14" s="56" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="56"/>
+      <c r="F14" s="56"/>
+      <c r="G14" s="56"/>
+      <c r="H14" s="56"/>
+      <c r="I14" s="56"/>
+      <c r="J14" s="56"/>
+      <c r="K14" s="56"/>
+      <c r="L14" s="56"/>
+      <c r="M14" s="56"/>
+      <c r="N14" s="56"/>
+      <c r="O14" s="56"/>
+      <c r="P14" s="56"/>
+      <c r="Q14" s="55"/>
       <c r="R14" s="25"/>
       <c r="S14" s="23"/>
       <c r="T14" s="23"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B15" s="26" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C15" s="27"/>
       <c r="D15" s="24" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="E15" s="24"/>
       <c r="F15" s="24"/>
@@ -7131,17 +7256,17 @@
       <c r="O15" s="24"/>
       <c r="P15" s="24"/>
       <c r="Q15" s="27"/>
-      <c r="R15" s="23"/>
+      <c r="R15" s="25"/>
       <c r="S15" s="23"/>
       <c r="T15" s="23"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B16" s="26" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C16" s="27"/>
       <c r="D16" s="24" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E16" s="24"/>
       <c r="F16" s="24"/>
@@ -7162,11 +7287,11 @@
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B17" s="26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17" s="27"/>
       <c r="D17" s="24" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E17" s="24"/>
       <c r="F17" s="24"/>
@@ -7182,16 +7307,16 @@
       <c r="P17" s="24"/>
       <c r="Q17" s="27"/>
       <c r="R17" s="23"/>
-      <c r="S17" s="25"/>
-      <c r="T17" s="25"/>
+      <c r="S17" s="23"/>
+      <c r="T17" s="23"/>
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B18" s="26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C18" s="27"/>
       <c r="D18" s="24" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E18" s="24"/>
       <c r="F18" s="24"/>
@@ -7212,11 +7337,11 @@
     </row>
     <row r="19" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B19" s="26" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="C19" s="27"/>
       <c r="D19" s="24" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E19" s="24"/>
       <c r="F19" s="24"/>
@@ -7232,40 +7357,61 @@
       <c r="P19" s="24"/>
       <c r="Q19" s="27"/>
       <c r="R19" s="23"/>
-      <c r="S19" s="23"/>
-      <c r="T19" s="23"/>
-    </row>
-    <row r="20" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="30"/>
-      <c r="D20" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="29"/>
-      <c r="J20" s="29"/>
-      <c r="K20" s="29"/>
-      <c r="L20" s="29"/>
-      <c r="M20" s="29"/>
-      <c r="N20" s="29"/>
-      <c r="O20" s="29"/>
-      <c r="P20" s="29"/>
-      <c r="Q20" s="30"/>
+      <c r="S19" s="25"/>
+      <c r="T19" s="25"/>
+    </row>
+    <row r="20" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B20" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="27"/>
+      <c r="D20" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24"/>
+      <c r="L20" s="24"/>
+      <c r="M20" s="24"/>
+      <c r="N20" s="24"/>
+      <c r="O20" s="24"/>
+      <c r="P20" s="24"/>
+      <c r="Q20" s="27"/>
       <c r="R20" s="23"/>
       <c r="S20" s="23"/>
       <c r="T20" s="23"/>
     </row>
-    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="30"/>
+      <c r="D21" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="29"/>
+      <c r="K21" s="29"/>
+      <c r="L21" s="29"/>
+      <c r="M21" s="29"/>
+      <c r="N21" s="29"/>
+      <c r="O21" s="29"/>
+      <c r="P21" s="29"/>
+      <c r="Q21" s="30"/>
       <c r="R21" s="23"/>
       <c r="S21" s="23"/>
       <c r="T21" s="23"/>
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="R22" s="23"/>
       <c r="S22" s="23"/>
       <c r="T22" s="23"/>
     </row>
@@ -7280,6 +7426,10 @@
     <row r="25" spans="2:20" x14ac:dyDescent="0.25">
       <c r="S25" s="23"/>
       <c r="T25" s="23"/>
+    </row>
+    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="S26" s="23"/>
+      <c r="T26" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -7309,7 +7459,7 @@
     </row>
     <row r="2" spans="2:19" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="51" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C2" s="52"/>
       <c r="D2" s="52"/>
@@ -7331,7 +7481,7 @@
     </row>
     <row r="3" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="35" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C3" s="36"/>
       <c r="D3" s="36"/>
@@ -7353,7 +7503,7 @@
     </row>
     <row r="4" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="35" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C4" s="36"/>
       <c r="D4" s="36"/>
@@ -7375,7 +7525,7 @@
     </row>
     <row r="5" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="35" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C5" s="36"/>
       <c r="D5" s="36"/>
@@ -7417,7 +7567,7 @@
     </row>
     <row r="7" spans="2:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="38" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C7" s="39"/>
       <c r="D7" s="39"/>
@@ -7508,7 +7658,7 @@
     </row>
     <row r="2" spans="2:19" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="59" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C2" s="60"/>
       <c r="D2" s="60"/>
@@ -7530,7 +7680,7 @@
     </row>
     <row r="3" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="41" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C3" s="42"/>
       <c r="D3" s="42"/>
@@ -7552,7 +7702,7 @@
     </row>
     <row r="4" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="41" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C4" s="42"/>
       <c r="D4" s="42"/>
@@ -7574,7 +7724,7 @@
     </row>
     <row r="5" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="41" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C5" s="42"/>
       <c r="D5" s="42"/>
@@ -7616,7 +7766,7 @@
     </row>
     <row r="7" spans="2:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="44" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C7" s="45"/>
       <c r="D7" s="45"/>
@@ -7735,7 +7885,7 @@
     <row r="2" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="20"/>
       <c r="B2" s="51" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C2" s="52"/>
       <c r="D2" s="52"/>
@@ -7760,7 +7910,7 @@
     <row r="3" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
       <c r="B3" s="35" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C3" s="36"/>
       <c r="D3" s="36"/>
@@ -7785,7 +7935,7 @@
     <row r="4" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20"/>
       <c r="B4" s="38" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C4" s="39"/>
       <c r="D4" s="39"/>
@@ -8058,7 +8208,7 @@
     </row>
     <row r="3" spans="2:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="35" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C3" s="36"/>
       <c r="D3" s="36"/>
@@ -8081,7 +8231,7 @@
     </row>
     <row r="4" spans="2:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="35" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C4" s="36"/>
       <c r="D4" s="36"/>
@@ -8125,7 +8275,7 @@
     </row>
     <row r="6" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="38" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C6" s="39"/>
       <c r="D6" s="39"/>
@@ -8278,8 +8428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9:I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8304,7 +8454,7 @@
     </row>
     <row r="2" spans="1:19" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="51" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C2" s="52"/>
       <c r="D2" s="52"/>
@@ -8326,7 +8476,7 @@
     </row>
     <row r="3" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="35" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C3" s="36"/>
       <c r="D3" s="36"/>
@@ -8348,7 +8498,7 @@
     </row>
     <row r="4" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="38" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C4" s="39"/>
       <c r="D4" s="39"/>
@@ -8467,7 +8617,7 @@
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
       <c r="H9" s="8"/>
-      <c r="I9" s="17"/>
+      <c r="I9" s="16"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B10" s="19" t="s">
@@ -8479,7 +8629,7 @@
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="8"/>
-      <c r="I10" s="17"/>
+      <c r="I10" s="16"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B11" s="12" t="s">
@@ -8515,7 +8665,7 @@
       <c r="H12" s="8">
         <v>10</v>
       </c>
-      <c r="I12" s="17">
+      <c r="I12" s="16">
         <v>0.1</v>
       </c>
     </row>
@@ -8529,7 +8679,7 @@
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="8"/>
-      <c r="I13" s="17"/>
+      <c r="I13" s="16"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B14" s="12" t="s">
@@ -8565,7 +8715,7 @@
       <c r="H15" s="8">
         <v>10</v>
       </c>
-      <c r="I15" s="17">
+      <c r="I15" s="16">
         <v>0.05</v>
       </c>
     </row>

</xml_diff>